<commit_message>
Editing and new MyWishlistTests
</commit_message>
<xml_diff>
--- a/Data/SeleniumFinalProject.xlsx
+++ b/Data/SeleniumFinalProject.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RedMonster\eclipse-workspace\FinalProject\SeleniumProject\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA61F48-69B2-435C-9324-E03626278801}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC7D2F7-F8CC-40D1-ACDE-DE21985FA748}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{F75050DC-36F9-4956-BD17-0ADEE7515C94}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{F75050DC-36F9-4956-BD17-0ADEE7515C94}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenario" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="126">
   <si>
     <t>Section</t>
   </si>
@@ -354,9 +354,6 @@
     <t>Current password is entered and it is not visible</t>
   </si>
   <si>
-    <t>Your personal information has been successfully updated.</t>
-  </si>
-  <si>
     <t>The notification "Your personal information has 
 been successfully updated."</t>
   </si>
@@ -392,6 +389,41 @@
   </si>
   <si>
     <t>Under the section for creating new wishlist there is a section with the information about the wish list that you have created</t>
+  </si>
+  <si>
+    <t>Precondition: The user is logged in/TC1-ID:1
+The user already has at least one wishlist</t>
+  </si>
+  <si>
+    <t>New collection</t>
+  </si>
+  <si>
+    <t>The table with the information of your wish list/s is present</t>
+  </si>
+  <si>
+    <t>Click on the "X" button in the lost column of the wishlist table</t>
+  </si>
+  <si>
+    <t>The alert message pop ups where you can confirm or cancel the removal of the wish list</t>
+  </si>
+  <si>
+    <t>Confirm the removal of the wishlist by clicking on the button "OK"</t>
+  </si>
+  <si>
+    <t>Precondition: The user is logged in/TC1-ID:1
+The user already has at least two wishlists</t>
+  </si>
+  <si>
+    <t>Find the table with the information of your wishlists</t>
+  </si>
+  <si>
+    <t>The wishlist is removed, the remaining wish list is visible and you can add new wishlist</t>
+  </si>
+  <si>
+    <t>Sandy Maven</t>
+  </si>
+  <si>
+    <t>Bell</t>
   </si>
 </sst>
 </file>
@@ -828,7 +860,7 @@
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -950,31 +982,31 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="E13" s="6"/>
     </row>
@@ -1369,8 +1401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E63A047-E3AB-4F76-8A40-CE3DEC8B9983}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1850,7 +1882,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
         <v>32</v>
       </c>
@@ -1859,6 +1891,9 @@
       </c>
       <c r="E38" s="12" t="s">
         <v>37</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
@@ -2107,7 +2142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B235CAD-2BD4-482A-9DAB-8116F8ACCF7E}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -2629,13 +2664,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D28EBA69-A8D6-4BC1-83C9-6BF53B471703}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.42578125" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" customWidth="1"/>
     <col min="3" max="3" width="42.85546875" customWidth="1"/>
     <col min="4" max="4" width="24.85546875" customWidth="1"/>
     <col min="5" max="5" width="57.140625" customWidth="1"/>
@@ -2690,7 +2725,9 @@
       <c r="C4" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="10" t="s">
         <v>11</v>
@@ -2734,13 +2771,15 @@
         <v>100</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F7" s="10"/>
+        <v>124</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
@@ -2748,11 +2787,13 @@
       <c r="C8" s="4"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="10"/>
+      <c r="F8" s="10" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -2782,10 +2823,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1FDE8B5-28E1-4953-A99F-1AEB82CAC5BE}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2802,7 +2843,7 @@
         <v>94</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -2839,10 +2880,10 @@
     <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -2853,13 +2894,13 @@
     <row r="5" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="10" t="s">
@@ -2872,21 +2913,191 @@
         <v>100</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="F6" s="10"/>
-    </row>
-    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="10"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="48" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="10" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updating tests and excel file
</commit_message>
<xml_diff>
--- a/Data/SeleniumFinalProject.xlsx
+++ b/Data/SeleniumFinalProject.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RedMonster\eclipse-workspace\FinalProject\SeleniumProject\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40051D72-87D7-4ECD-BBF7-F18CC994DF8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE865CF-6785-4628-BCCF-83F5230897ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{F75050DC-36F9-4956-BD17-0ADEE7515C94}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{F75050DC-36F9-4956-BD17-0ADEE7515C94}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenario" sheetId="1" r:id="rId1"/>
-    <sheet name="TC1" sheetId="2" r:id="rId2"/>
-    <sheet name="TC2" sheetId="3" r:id="rId3"/>
-    <sheet name="TC3" sheetId="4" r:id="rId4"/>
-    <sheet name="TC4" sheetId="5" r:id="rId5"/>
+    <sheet name="Login" sheetId="2" r:id="rId2"/>
+    <sheet name="MyAddress" sheetId="3" r:id="rId3"/>
+    <sheet name="MyPersonalInformation" sheetId="4" r:id="rId4"/>
+    <sheet name="Wishlist" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="128">
   <si>
     <t>Section</t>
   </si>
@@ -83,22 +83,13 @@
     <t>Login section</t>
   </si>
   <si>
-    <t>TC1</t>
-  </si>
-  <si>
     <t>Verify that you can login with valid credentials</t>
   </si>
   <si>
-    <t>TC2</t>
-  </si>
-  <si>
     <t>Verify that you can not login with empty credentials</t>
   </si>
   <si>
     <t>Verify that you can log out</t>
-  </si>
-  <si>
-    <t>Go to the "http://automationpractice.com/index.php/"</t>
   </si>
   <si>
     <t>The page opens</t>
@@ -151,9 +142,6 @@
     <t>mark.johanson@fakemail.com</t>
   </si>
   <si>
-    <t>There is 1 error</t>
-  </si>
-  <si>
     <t>ID:3</t>
   </si>
   <si>
@@ -294,12 +282,6 @@
     <t>Verify that you can not login with invalid password</t>
   </si>
   <si>
-    <t>Precondition: The user is logged in/TC1-ID:1</t>
-  </si>
-  <si>
-    <t>Precondition:The user is logged in/TC1-ID:1</t>
-  </si>
-  <si>
     <t>ID:9</t>
   </si>
   <si>
@@ -315,16 +297,10 @@
     <t>The address is deleted and the other address is visible</t>
   </si>
   <si>
-    <t>Precondition: The user is logged in/TC1-ID:1; There are two addresses at the profile</t>
-  </si>
-  <si>
     <t>My Personal Information</t>
   </si>
   <si>
     <t>Verify that you can edit your personal information</t>
-  </si>
-  <si>
-    <t>TC3</t>
   </si>
   <si>
     <t>ID:10</t>
@@ -367,9 +343,6 @@
     <t>Verify that you can remove wish list</t>
   </si>
   <si>
-    <t>TC4</t>
-  </si>
-  <si>
     <t>Click on the section "MY WISHLIST"</t>
   </si>
   <si>
@@ -391,42 +364,75 @@
     <t>Under the section for creating new wishlist there is a section with the information about the wish list that you have created</t>
   </si>
   <si>
-    <t>Precondition: The user is logged in/TC1-ID:1
+    <t>New collection</t>
+  </si>
+  <si>
+    <t>The table with the information of your wish list/s is present</t>
+  </si>
+  <si>
+    <t>Click on the "X" button in the lost column of the wishlist table</t>
+  </si>
+  <si>
+    <t>The alert message pop ups where you can confirm or cancel the removal of the wish list</t>
+  </si>
+  <si>
+    <t>Confirm the removal of the wishlist by clicking on the button "OK"</t>
+  </si>
+  <si>
+    <t>Find the table with the information of your wishlists</t>
+  </si>
+  <si>
+    <t>The wishlist is removed, the remaining wish list is visible and you can add new wishlist</t>
+  </si>
+  <si>
+    <t>Sandy Maven</t>
+  </si>
+  <si>
+    <t>Bell</t>
+  </si>
+  <si>
+    <t>Sandy Bell</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>MyAddress</t>
+  </si>
+  <si>
+    <t>MyPersonalInformation</t>
+  </si>
+  <si>
+    <t>Wishlist</t>
+  </si>
+  <si>
+    <t>Precondition: The user is logged in
+The user has one address</t>
+  </si>
+  <si>
+    <t>Precondition: The user is logged in 
+There are two addresses at the profile</t>
+  </si>
+  <si>
+    <t>Precondition: The user is logged in</t>
+  </si>
+  <si>
+    <t>Precondition: The user is logged in
 The user already has at least one wishlist</t>
   </si>
   <si>
-    <t>New collection</t>
-  </si>
-  <si>
-    <t>The table with the information of your wish list/s is present</t>
-  </si>
-  <si>
-    <t>Click on the "X" button in the lost column of the wishlist table</t>
-  </si>
-  <si>
-    <t>The alert message pop ups where you can confirm or cancel the removal of the wish list</t>
-  </si>
-  <si>
-    <t>Confirm the removal of the wishlist by clicking on the button "OK"</t>
-  </si>
-  <si>
-    <t>Precondition: The user is logged in/TC1-ID:1
-The user already has at least two wishlists</t>
-  </si>
-  <si>
-    <t>Find the table with the information of your wishlists</t>
-  </si>
-  <si>
-    <t>The wishlist is removed, the remaining wish list is visible and you can add new wishlist</t>
-  </si>
-  <si>
-    <t>Sandy Maven</t>
-  </si>
-  <si>
-    <t>Bell</t>
-  </si>
-  <si>
-    <t>Sandy Bell</t>
+    <t>Precondition: The user is logged in
+The user has two wishlists</t>
+  </si>
+  <si>
+    <t>Precondition:The user is logged in
+The user has one address</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/index.php</t>
+  </si>
+  <si>
+    <t>Go to the URL</t>
   </si>
 </sst>
 </file>
@@ -513,7 +519,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -545,6 +551,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -863,14 +872,14 @@
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="41.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
@@ -897,119 +906,119 @@
         <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>17</v>
+        <v>117</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>17</v>
+        <v>117</v>
       </c>
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>17</v>
+        <v>117</v>
       </c>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="E13" s="6"/>
     </row>
@@ -1404,8 +1413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E63A047-E3AB-4F76-8A40-CE3DEC8B9983}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1413,7 +1422,8 @@
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="46.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="50" style="3" customWidth="1"/>
-    <col min="4" max="5" width="27.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="33" style="3" customWidth="1"/>
     <col min="6" max="6" width="23" style="3" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" customWidth="1"/>
     <col min="8" max="8" width="20.140625" customWidth="1"/>
@@ -1425,7 +1435,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -1436,7 +1446,7 @@
     <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -1480,10 +1490,13 @@
     </row>
     <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>11</v>
@@ -1493,10 +1506,10 @@
     </row>
     <row r="6" spans="1:8" ht="48" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>11</v>
@@ -1504,10 +1517,10 @@
     </row>
     <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>11</v>
@@ -1515,13 +1528,13 @@
     </row>
     <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>11</v>
@@ -1529,13 +1542,13 @@
     </row>
     <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>11</v>
@@ -1543,10 +1556,10 @@
     </row>
     <row r="10" spans="1:8" ht="48" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>11</v>
@@ -1554,10 +1567,10 @@
     </row>
     <row r="11" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -1566,7 +1579,7 @@
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -1604,10 +1617,13 @@
     </row>
     <row r="15" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>11</v>
@@ -1615,10 +1631,10 @@
     </row>
     <row r="16" spans="1:8" ht="48" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>11</v>
@@ -1626,10 +1642,10 @@
     </row>
     <row r="17" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>11</v>
@@ -1637,13 +1653,13 @@
     </row>
     <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>11</v>
@@ -1651,13 +1667,13 @@
     </row>
     <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="D19" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>11</v>
@@ -1665,24 +1681,22 @@
     </row>
     <row r="20" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>37</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="E20" s="13"/>
       <c r="F20" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -1691,7 +1705,7 @@
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -1729,10 +1743,13 @@
     </row>
     <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="F25" s="10" t="s">
         <v>11</v>
@@ -1740,10 +1757,10 @@
     </row>
     <row r="26" spans="1:6" ht="48" x14ac:dyDescent="0.3">
       <c r="B26" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F26" s="10" t="s">
         <v>11</v>
@@ -1751,10 +1768,10 @@
     </row>
     <row r="27" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F27" s="10" t="s">
         <v>11</v>
@@ -1762,13 +1779,13 @@
     </row>
     <row r="28" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>11</v>
@@ -1776,13 +1793,13 @@
     </row>
     <row r="29" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="D29" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>11</v>
@@ -1790,24 +1807,22 @@
     </row>
     <row r="30" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>37</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="E30" s="13"/>
       <c r="F30" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
@@ -1816,7 +1831,7 @@
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -1854,10 +1869,13 @@
     </row>
     <row r="35" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="F35" s="10" t="s">
         <v>11</v>
@@ -1865,10 +1883,10 @@
     </row>
     <row r="36" spans="1:6" ht="48" x14ac:dyDescent="0.3">
       <c r="B36" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F36" s="10" t="s">
         <v>11</v>
@@ -1876,10 +1894,10 @@
     </row>
     <row r="37" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F37" s="10" t="s">
         <v>11</v>
@@ -1887,24 +1905,22 @@
     </row>
     <row r="38" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>37</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="E38" s="13"/>
       <c r="F38" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
@@ -1913,7 +1929,7 @@
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
       <c r="B40" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
@@ -1951,10 +1967,13 @@
     </row>
     <row r="43" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B43" s="3" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="F43" s="10" t="s">
         <v>11</v>
@@ -1962,10 +1981,10 @@
     </row>
     <row r="44" spans="1:6" ht="48" x14ac:dyDescent="0.3">
       <c r="B44" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F44" s="10" t="s">
         <v>11</v>
@@ -1973,10 +1992,10 @@
     </row>
     <row r="45" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B45" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F45" s="10" t="s">
         <v>11</v>
@@ -1984,24 +2003,22 @@
     </row>
     <row r="46" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="B46" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>37</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="E46" s="12"/>
       <c r="F46" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
@@ -2010,7 +2027,7 @@
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
       <c r="B48" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
@@ -2048,10 +2065,13 @@
     </row>
     <row r="51" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B51" s="3" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="F51" s="10" t="s">
         <v>11</v>
@@ -2059,10 +2079,10 @@
     </row>
     <row r="52" spans="1:6" ht="48" x14ac:dyDescent="0.3">
       <c r="B52" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>11</v>
@@ -2070,10 +2090,10 @@
     </row>
     <row r="53" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B53" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>11</v>
@@ -2081,13 +2101,13 @@
     </row>
     <row r="54" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B54" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>11</v>
@@ -2095,13 +2115,13 @@
     </row>
     <row r="55" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B55" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="D55" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>11</v>
@@ -2109,10 +2129,10 @@
     </row>
     <row r="56" spans="1:6" ht="48" x14ac:dyDescent="0.3">
       <c r="B56" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F56" s="10" t="s">
         <v>11</v>
@@ -2120,10 +2140,10 @@
     </row>
     <row r="57" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="B57" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F57" s="10" t="s">
         <v>11</v>
@@ -2145,8 +2165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B235CAD-2BD4-482A-9DAB-8116F8ACCF7E}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2160,19 +2180,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -2200,10 +2220,10 @@
     <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -2214,10 +2234,10 @@
     <row r="5" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -2228,13 +2248,13 @@
     <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="10" t="s">
@@ -2244,14 +2264,14 @@
     <row r="7" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>11</v>
@@ -2260,10 +2280,10 @@
     <row r="8" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -2272,13 +2292,13 @@
     <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="10"/>
@@ -2286,32 +2306,32 @@
     <row r="10" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F10" s="10"/>
     </row>
     <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="4" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -2339,10 +2359,10 @@
     <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -2353,10 +2373,10 @@
     <row r="15" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -2367,13 +2387,13 @@
     <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="10" t="s">
@@ -2383,13 +2403,13 @@
     <row r="17" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="10" t="s">
@@ -2399,10 +2419,10 @@
     <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -2413,10 +2433,10 @@
     <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D19" s="3">
         <v>21458</v>
@@ -2429,10 +2449,10 @@
     <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D20" s="3">
         <v>456156423</v>
@@ -2445,13 +2465,13 @@
     <row r="21" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="10" t="s">
@@ -2461,14 +2481,14 @@
     <row r="22" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>11</v>
@@ -2476,10 +2496,10 @@
     </row>
     <row r="23" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -2488,7 +2508,7 @@
     <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="4" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -2516,10 +2536,10 @@
     <row r="26" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -2530,10 +2550,10 @@
     <row r="27" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -2544,10 +2564,10 @@
     <row r="28" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -2669,7 +2689,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2684,19 +2704,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
     </row>
-    <row r="2" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -2724,16 +2744,16 @@
     <row r="4" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>11</v>
@@ -2742,13 +2762,13 @@
     <row r="5" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="10" t="s">
@@ -2758,13 +2778,13 @@
     <row r="6" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="10" t="s">
@@ -2774,14 +2794,14 @@
     <row r="7" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="4" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>11</v>
@@ -2831,8 +2851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1FDE8B5-28E1-4953-A99F-1AEB82CAC5BE}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2846,10 +2866,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -2858,7 +2878,7 @@
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -2886,10 +2906,10 @@
     <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -2900,13 +2920,13 @@
     <row r="5" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="10" t="s">
@@ -2916,10 +2936,10 @@
     <row r="6" spans="1:6" ht="48" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -2929,10 +2949,10 @@
     </row>
     <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -2941,7 +2961,7 @@
     <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="4" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -2969,10 +2989,10 @@
     <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -2983,13 +3003,13 @@
     <row r="11" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="4" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="10" t="s">
@@ -2999,10 +3019,10 @@
     <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -3012,10 +3032,10 @@
     </row>
     <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -3024,7 +3044,7 @@
     <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="4" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -3052,10 +3072,10 @@
     <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -3066,10 +3086,10 @@
     <row r="17" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -3080,10 +3100,10 @@
     <row r="18" spans="1:6" ht="48" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -3094,10 +3114,10 @@
     <row r="19" spans="1:6" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="4" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>

</xml_diff>